<commit_message>
Feat : Object Pool 변경 (tag -> ID)
</commit_message>
<xml_diff>
--- a/Assets/Excel/Projectile/ProjectileDB_Sheet.xlsx
+++ b/Assets/Excel/Projectile/ProjectileDB_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\Projectile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D65E09-B79B-449B-9D8A-BC100BDA3162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA1E273-E27D-4B80-AA3B-75DAC3B24F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{6AD199CF-C248-492C-9CAC-526C1675E22C}"/>
   </bookViews>
@@ -46,11 +46,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Resources/Projectile/Orange Explosion</t>
+    <t>Projectile/Prefabs/Orange Explosion</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Resources/Projectile/Poison</t>
+    <t>Projectile/Prefabs/Poison</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -467,7 +467,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Feat : Projectile 임시 병합
</commit_message>
<xml_diff>
--- a/Assets/Excel/Projectile/ProjectileDB_Sheet.xlsx
+++ b/Assets/Excel/Projectile/ProjectileDB_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\Projectile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA1E273-E27D-4B80-AA3B-75DAC3B24F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4198F417-89B6-430F-B81E-C48FE4352BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{6AD199CF-C248-492C-9CAC-526C1675E22C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,6 +51,32 @@
   </si>
   <si>
     <t>Projectile/Prefabs/Poison</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>speed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Magic</t>
+  </si>
+  <si>
+    <t>Magic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DamageType</t>
+  </si>
+  <si>
+    <t>Physical</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>속도는 Speed * 1.n으로 조절하면 될듯</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -92,7 +118,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,6 +128,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -120,14 +152,23 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -464,50 +505,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F2F97B-EEE6-4097-B645-8ABD2F571A0C}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>40000000</v>
       </c>
+      <c r="F2" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>40000001</v>
       </c>
+      <c r="F3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>40000100</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>40000101</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>